<commit_message>
Photo sizing + docs + SEO updates
</commit_message>
<xml_diff>
--- a/docs/0 south ave land comps.xlsx
+++ b/docs/0 south ave land comps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f65a642d0762be/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3f65a642d0762be/Desktop/214_assets/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{44F1ADE8-0AC1-47FA-B9F9-49DC3BFBA221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE2026B1-6ECD-4C49-9D36-F9ED62D473A7}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="8_{44F1ADE8-0AC1-47FA-B9F9-49DC3BFBA221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DB94E68-6C08-4853-BC00-F76C46D5159D}"/>
   <bookViews>
-    <workbookView xWindow="11052" yWindow="0" windowWidth="12084" windowHeight="9000" xr2:uid="{B79E797B-7245-4FDD-B2DA-DA87448AFCEC}"/>
+    <workbookView xWindow="2124" yWindow="600" windowWidth="20004" windowHeight="11640" xr2:uid="{B79E797B-7245-4FDD-B2DA-DA87448AFCEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -227,12 +233,16 @@
     <xf numFmtId="6" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +585,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="C13" sqref="C13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,28 +984,28 @@
       <c r="B13" s="10">
         <v>100</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="11">
         <v>6</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="11">
         <v>6.9199999999999998E-2</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="12">
         <v>3016</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="I13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1094,5 +1104,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>